<commit_message>
Colocando enlaces al repositorio
</commit_message>
<xml_diff>
--- a/TrabajoAutonomoRefactoring.xlsx
+++ b/TrabajoAutonomoRefactoring.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="143">
   <si>
     <t>Code Smell</t>
   </si>
@@ -412,12 +412,87 @@
   <si>
     <t>switch statement in java. Retrieved from https://www.tutorialspoint.com/java/switch_statement_in_java.htm</t>
   </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Bloaters/dataClumps/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Bloaters/dataClumps/Refactoring</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Bloaters/largeClass/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Bloaters/largeClass/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Bloaters/longMethod/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Bloaters/longMethod/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Bloaters/primitiveObsession/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Bloaters/primitiveObsession/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/ObjectOrientationAbusers/SwitchStatements/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/ObjectOrientationAbusers/SwitchStatements/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/ObjectOrientationAbusers/RefusedBequest/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/ObjectOrientationAbusers/RefusedBequest/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/ChangePreventers/ShotgunSurgery/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/ChangePreventers/ShotgunSurgery/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Dispensables/Comments/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Dispensables/Comments/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Dispensables/DuplicateCode/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Dispensables/DuplicateCode/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Dispensables/DataClass/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Dispensables/DataClass/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Couplers/FeatureEnvy/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Couplers/FeatureEnvy/Refactoring</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Couplers/InappropriateIntimacy/codeSmell</t>
+  </si>
+  <si>
+    <t>https://github.com/ginpajac/TrabajoAutonomoRefactoring/tree/master/CodeSmells/src/Couplers/InappropriateIntimacy/Refactoring</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -529,6 +604,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -609,26 +692,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="hair">
         <color theme="0"/>
       </left>
@@ -926,17 +989,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashed">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -963,7 +1015,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="hair">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -973,199 +1027,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1179,8 +1149,153 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="29" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1466,8 +1581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1480,750 +1596,801 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="73"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="77" t="s">
+      <c r="A2" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="69" t="s">
+      <c r="A3" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="71"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="43"/>
     </row>
     <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="63" t="s">
+      <c r="B4" s="34"/>
+      <c r="C4" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="67" t="s">
+      <c r="E4" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="7"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="39" t="s">
+      <c r="C5" s="36"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="56" t="s">
+      <c r="C7" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="17"/>
+      <c r="E7" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="F7" s="68" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="26" t="s">
+      <c r="A8" s="44"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="17"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="68"/>
     </row>
     <row r="9" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="26" t="s">
+      <c r="A9" s="44"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="17"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="68"/>
     </row>
     <row r="10" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="49"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="26" t="s">
+      <c r="A10" s="44"/>
+      <c r="B10" s="46"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="17"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="68"/>
     </row>
     <row r="11" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="26" t="s">
+      <c r="A11" s="44"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="48"/>
+      <c r="D11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="17"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="68"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="50"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="28" t="s">
+      <c r="A12" s="45"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="69"/>
     </row>
     <row r="13" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
+      <c r="E13" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="63" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="47"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="26" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="46"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="17"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="61"/>
     </row>
     <row r="15" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="47"/>
-      <c r="B15" s="49"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="26" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="46"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="17"/>
+      <c r="E15" s="58"/>
+      <c r="F15" s="61"/>
     </row>
     <row r="16" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="30" t="s">
+      <c r="A16" s="45"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
-    </row>
-    <row r="17" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51" t="s">
+      <c r="E16" s="64"/>
+      <c r="F16" s="70"/>
+    </row>
+    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="31" t="s">
+      <c r="D17" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="32" t="s">
+      <c r="E17" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="17"/>
-    </row>
-    <row r="19" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="47"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="32" t="s">
+      <c r="E18" s="71"/>
+      <c r="F18" s="61"/>
+    </row>
+    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="44"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="17"/>
-    </row>
-    <row r="20" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="47"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="32" t="s">
+      <c r="E19" s="71"/>
+      <c r="F19" s="61"/>
+    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="44"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="17"/>
-    </row>
-    <row r="21" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="47"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="32" t="s">
+      <c r="E20" s="71"/>
+      <c r="F20" s="61"/>
+    </row>
+    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="44"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="17"/>
-    </row>
-    <row r="22" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="47"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="32" t="s">
+      <c r="E21" s="71"/>
+      <c r="F21" s="61"/>
+    </row>
+    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="44"/>
+      <c r="B22" s="46"/>
+      <c r="C22" s="48"/>
+      <c r="D22" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E22" s="8"/>
-      <c r="F22" s="17"/>
-    </row>
-    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="58"/>
-      <c r="D23" s="30" t="s">
+      <c r="E22" s="71"/>
+      <c r="F22" s="61"/>
+    </row>
+    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="45"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="49"/>
+      <c r="D23" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-    </row>
-    <row r="24" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="51" t="s">
+      <c r="E23" s="72"/>
+      <c r="F23" s="70"/>
+    </row>
+    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="53" t="s">
+      <c r="B24" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="55" t="s">
+      <c r="C24" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="D24" s="32" t="s">
+      <c r="D24" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="17"/>
-    </row>
-    <row r="25" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="49"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="32" t="s">
+      <c r="E24" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="63" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="44"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="17"/>
-    </row>
-    <row r="26" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="52"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="61"/>
+      <c r="G25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="55"/>
       <c r="B26" s="54"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="33" t="s">
+      <c r="C26" s="53"/>
+      <c r="D26" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="E26" s="59"/>
+      <c r="F26" s="62"/>
+    </row>
+    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="5"/>
-    </row>
-    <row r="28" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="47" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="49" t="s">
+      <c r="B28" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
-      <c r="B29" s="49"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="26" t="s">
+      <c r="E28" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="F28" s="68" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="44"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="26" t="s">
+      <c r="E29" s="71"/>
+      <c r="F29" s="73"/>
+    </row>
+    <row r="30" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="44"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
-      <c r="B31" s="49"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="26" t="s">
+      <c r="E30" s="71"/>
+      <c r="F30" s="73"/>
+    </row>
+    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="44"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="56"/>
-      <c r="D32" s="26" t="s">
+      <c r="E31" s="71"/>
+      <c r="F31" s="73"/>
+    </row>
+    <row r="32" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="44"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="6"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="73"/>
     </row>
     <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
-      <c r="B33" s="50"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="30" t="s">
+      <c r="A33" s="45"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="23"/>
-      <c r="F33" s="24"/>
+      <c r="E33" s="72"/>
+      <c r="F33" s="74"/>
     </row>
     <row r="34" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="51" t="s">
+      <c r="A34" s="50" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="53" t="s">
+      <c r="B34" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="6"/>
+      <c r="E34" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="63" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="35" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
+      <c r="A35" s="55"/>
       <c r="B35" s="54"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="26" t="s">
+      <c r="C35" s="53"/>
+      <c r="D35" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="6"/>
+      <c r="E35" s="53"/>
+      <c r="F35" s="75"/>
     </row>
     <row r="36" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="10"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="47" t="s">
+      <c r="A37" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="49" t="s">
+      <c r="B37" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="59" t="s">
+      <c r="C37" s="56" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="34" t="s">
+      <c r="D37" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27"/>
+      <c r="E37" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="F37" s="78" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="38" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="52"/>
+      <c r="A38" s="55"/>
       <c r="B38" s="54"/>
-      <c r="C38" s="60"/>
-      <c r="D38" s="26" t="s">
+      <c r="C38" s="57"/>
+      <c r="D38" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="27"/>
+      <c r="E38" s="57"/>
+      <c r="F38" s="77"/>
     </row>
     <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="25" t="s">
+      <c r="A39" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="10"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="B40" s="49" t="s">
+      <c r="B40" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="56" t="s">
+      <c r="C40" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D40" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="6"/>
+      <c r="E40" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="68" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
-      <c r="B41" s="49"/>
-      <c r="C41" s="56"/>
-      <c r="D41" s="26" t="s">
+      <c r="A41" s="44"/>
+      <c r="B41" s="46"/>
+      <c r="C41" s="48"/>
+      <c r="D41" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="6"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="68"/>
     </row>
     <row r="42" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="47"/>
-      <c r="B42" s="49"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="26" t="s">
+      <c r="A42" s="44"/>
+      <c r="B42" s="46"/>
+      <c r="C42" s="48"/>
+      <c r="D42" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="6"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="68"/>
     </row>
     <row r="43" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="48"/>
-      <c r="B43" s="50"/>
-      <c r="C43" s="58"/>
-      <c r="D43" s="28" t="s">
+      <c r="A43" s="45"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E43" s="23"/>
-      <c r="F43" s="24"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="69"/>
     </row>
     <row r="44" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="51" t="s">
+      <c r="A44" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="53" t="s">
+      <c r="B44" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="55" t="s">
+      <c r="C44" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="45" t="s">
+      <c r="D44" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="36"/>
+      <c r="E44" s="60" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44" s="63" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="45" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="47"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="56"/>
-      <c r="D45" s="34" t="s">
+      <c r="A45" s="44"/>
+      <c r="B45" s="46"/>
+      <c r="C45" s="48"/>
+      <c r="D45" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E45" s="14"/>
-      <c r="F45" s="3"/>
+      <c r="E45" s="71"/>
+      <c r="F45" s="68"/>
     </row>
     <row r="46" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="47"/>
-      <c r="B46" s="49"/>
-      <c r="C46" s="56"/>
-      <c r="D46" s="43" t="s">
+      <c r="A46" s="44"/>
+      <c r="B46" s="46"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="E46" s="14"/>
-      <c r="F46" s="3"/>
+      <c r="E46" s="71"/>
+      <c r="F46" s="68"/>
     </row>
     <row r="47" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="47"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="56"/>
-      <c r="D47" s="26" t="s">
+      <c r="A47" s="44"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="48"/>
+      <c r="D47" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E47" s="14"/>
-      <c r="F47" s="3"/>
+      <c r="E47" s="71"/>
+      <c r="F47" s="68"/>
     </row>
     <row r="48" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="47"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="56"/>
-      <c r="D48" s="26" t="s">
+      <c r="A48" s="44"/>
+      <c r="B48" s="46"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E48" s="14"/>
-      <c r="F48" s="3"/>
+      <c r="E48" s="71"/>
+      <c r="F48" s="68"/>
     </row>
     <row r="49" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
-      <c r="B49" s="49"/>
-      <c r="C49" s="56"/>
-      <c r="D49" s="26" t="s">
+      <c r="A49" s="44"/>
+      <c r="B49" s="46"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="14"/>
-      <c r="F49" s="3"/>
+      <c r="E49" s="71"/>
+      <c r="F49" s="68"/>
     </row>
     <row r="50" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="47"/>
-      <c r="B50" s="49"/>
-      <c r="C50" s="56"/>
-      <c r="D50" s="26" t="s">
+      <c r="A50" s="44"/>
+      <c r="B50" s="46"/>
+      <c r="C50" s="48"/>
+      <c r="D50" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="14"/>
-      <c r="F50" s="3"/>
+      <c r="E50" s="71"/>
+      <c r="F50" s="68"/>
     </row>
     <row r="51" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
-      <c r="B51" s="49"/>
-      <c r="C51" s="56"/>
-      <c r="D51" s="43" t="s">
+      <c r="A51" s="44"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="48"/>
+      <c r="D51" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E51" s="14"/>
-      <c r="F51" s="3"/>
+      <c r="E51" s="71"/>
+      <c r="F51" s="68"/>
     </row>
     <row r="52" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="47"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="56"/>
-      <c r="D52" s="26" t="s">
+      <c r="A52" s="44"/>
+      <c r="B52" s="46"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="14"/>
-      <c r="F52" s="3"/>
+      <c r="E52" s="71"/>
+      <c r="F52" s="68"/>
     </row>
     <row r="53" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="47"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="56"/>
-      <c r="D53" s="26" t="s">
+      <c r="A53" s="44"/>
+      <c r="B53" s="46"/>
+      <c r="C53" s="48"/>
+      <c r="D53" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E53" s="14"/>
-      <c r="F53" s="3"/>
+      <c r="E53" s="71"/>
+      <c r="F53" s="68"/>
     </row>
     <row r="54" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="47"/>
-      <c r="B54" s="49"/>
-      <c r="C54" s="56"/>
-      <c r="D54" s="26" t="s">
+      <c r="A54" s="44"/>
+      <c r="B54" s="46"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E54" s="14"/>
-      <c r="F54" s="3"/>
+      <c r="E54" s="71"/>
+      <c r="F54" s="68"/>
     </row>
     <row r="55" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="48"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="28" t="s">
+      <c r="A55" s="45"/>
+      <c r="B55" s="47"/>
+      <c r="C55" s="49"/>
+      <c r="D55" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="E55" s="37"/>
-      <c r="F55" s="38"/>
+      <c r="E55" s="72"/>
+      <c r="F55" s="69"/>
     </row>
     <row r="56" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="51" t="s">
+      <c r="A56" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="55" t="s">
+      <c r="C56" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="D56" s="32" t="s">
+      <c r="D56" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="E56" s="14"/>
-      <c r="F56" s="3"/>
+      <c r="E56" s="60" t="s">
+        <v>137</v>
+      </c>
+      <c r="F56" s="63" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="47"/>
-      <c r="B57" s="49"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="32" t="s">
+      <c r="A57" s="44"/>
+      <c r="B57" s="46"/>
+      <c r="C57" s="48"/>
+      <c r="D57" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="E57" s="14"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="71"/>
+      <c r="F57" s="73"/>
     </row>
     <row r="58" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="52"/>
+      <c r="A58" s="55"/>
       <c r="B58" s="54"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="44" t="s">
+      <c r="C58" s="53"/>
+      <c r="D58" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="E58" s="15"/>
-      <c r="F58" s="4"/>
+      <c r="E58" s="79"/>
+      <c r="F58" s="80"/>
     </row>
     <row r="59" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="25" t="s">
+      <c r="A59" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B59" s="16" t="s">
+      <c r="B59" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C59" s="11"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="16"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="8"/>
+      <c r="E59" s="8"/>
       <c r="F59" s="2"/>
     </row>
     <row r="60" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="47" t="s">
+      <c r="A60" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="B60" s="49" t="s">
+      <c r="B60" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C60" s="56" t="s">
+      <c r="C60" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="D60" s="26" t="s">
+      <c r="D60" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="14"/>
-      <c r="F60" s="3"/>
+      <c r="E60" s="71" t="s">
+        <v>139</v>
+      </c>
+      <c r="F60" s="68" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="48"/>
-      <c r="B61" s="50"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="28" t="s">
+      <c r="A61" s="45"/>
+      <c r="B61" s="47"/>
+      <c r="C61" s="49"/>
+      <c r="D61" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="E61" s="37"/>
-      <c r="F61" s="38"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="69"/>
     </row>
     <row r="62" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="51" t="s">
+      <c r="A62" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B62" s="53" t="s">
+      <c r="B62" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="C62" s="55" t="s">
+      <c r="C62" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="D62" s="26" t="s">
+      <c r="D62" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E62" s="14"/>
-      <c r="F62" s="3"/>
+      <c r="E62" s="60" t="s">
+        <v>141</v>
+      </c>
+      <c r="F62" s="63" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="47"/>
-      <c r="B63" s="49"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="26" t="s">
+      <c r="A63" s="44"/>
+      <c r="B63" s="46"/>
+      <c r="C63" s="48"/>
+      <c r="D63" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E63" s="14"/>
-      <c r="F63" s="3"/>
+      <c r="E63" s="71"/>
+      <c r="F63" s="73"/>
     </row>
     <row r="64" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="47"/>
-      <c r="B64" s="49"/>
-      <c r="C64" s="56"/>
-      <c r="D64" s="26" t="s">
+      <c r="A64" s="44"/>
+      <c r="B64" s="46"/>
+      <c r="C64" s="48"/>
+      <c r="D64" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E64" s="14"/>
-      <c r="F64" s="3"/>
+      <c r="E64" s="71"/>
+      <c r="F64" s="73"/>
     </row>
     <row r="65" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="52"/>
+      <c r="A65" s="55"/>
       <c r="B65" s="54"/>
-      <c r="C65" s="57"/>
-      <c r="D65" s="33" t="s">
+      <c r="C65" s="53"/>
+      <c r="D65" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="E65" s="15"/>
-      <c r="F65" s="4"/>
+      <c r="E65" s="79"/>
+      <c r="F65" s="80"/>
     </row>
     <row r="66" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
@@ -2242,28 +2409,28 @@
       <c r="F67" s="1"/>
     </row>
     <row r="68" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="78" t="s">
+      <c r="A68" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B68" s="74"/>
-      <c r="C68" s="74"/>
-      <c r="D68" s="74"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="74"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="75"/>
-      <c r="J68" s="75"/>
-      <c r="K68" s="75"/>
-      <c r="L68" s="75"/>
-      <c r="M68" s="75"/>
-      <c r="N68" s="75"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="28"/>
+      <c r="F68" s="28"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="29"/>
+      <c r="K68" s="29"/>
+      <c r="L68" s="29"/>
+      <c r="M68" s="29"/>
+      <c r="N68" s="29"/>
     </row>
     <row r="69" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="B69" s="25" t="s">
         <v>112</v>
       </c>
       <c r="C69" s="1"/>
@@ -2274,7 +2441,7 @@
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="46" t="s">
+      <c r="B70" s="25" t="s">
         <v>103</v>
       </c>
       <c r="C70" s="1"/>
@@ -2286,7 +2453,7 @@
       <c r="A71" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B71" s="46" t="s">
+      <c r="B71" s="25" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="1"/>
@@ -2298,7 +2465,7 @@
       <c r="A72" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="25" t="s">
         <v>106</v>
       </c>
       <c r="C72" s="1"/>
@@ -2334,7 +2501,7 @@
       <c r="A75" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B75" s="46" t="s">
+      <c r="B75" s="25" t="s">
         <v>110</v>
       </c>
       <c r="C75" s="1"/>
@@ -2370,7 +2537,7 @@
       <c r="A78" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B78" s="46" t="s">
+      <c r="B78" s="25" t="s">
         <v>113</v>
       </c>
       <c r="C78" s="1"/>
@@ -2382,7 +2549,7 @@
       <c r="A79" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B79" s="46" t="s">
+      <c r="B79" s="25" t="s">
         <v>115</v>
       </c>
       <c r="C79" s="1"/>
@@ -2394,7 +2561,7 @@
       <c r="A80" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B80" s="46" t="s">
+      <c r="B80" s="25" t="s">
         <v>117</v>
       </c>
       <c r="C80" s="1"/>
@@ -2811,50 +2978,100 @@
       <c r="F131" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A3:F3"/>
+  <mergeCells count="65">
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="E62:E65"/>
+    <mergeCell ref="F62:F65"/>
+    <mergeCell ref="E40:E43"/>
+    <mergeCell ref="F40:F43"/>
+    <mergeCell ref="E44:E55"/>
+    <mergeCell ref="F44:F55"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="E28:E33"/>
+    <mergeCell ref="F28:F33"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="F34:F35"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="E7:E12"/>
+    <mergeCell ref="F7:F12"/>
+    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="F13:F16"/>
+    <mergeCell ref="E17:E23"/>
+    <mergeCell ref="F17:F23"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="A62:A65"/>
+    <mergeCell ref="B62:B65"/>
+    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="C44:C55"/>
+    <mergeCell ref="A44:A55"/>
+    <mergeCell ref="B44:B55"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="C40:C43"/>
+    <mergeCell ref="A28:A33"/>
+    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="C28:C33"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="B17:B23"/>
+    <mergeCell ref="C17:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A24:A26"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="B7:B12"/>
     <mergeCell ref="C7:C12"/>
     <mergeCell ref="A13:A16"/>
     <mergeCell ref="B13:B16"/>
     <mergeCell ref="C13:C16"/>
-    <mergeCell ref="A17:A23"/>
-    <mergeCell ref="B17:B23"/>
-    <mergeCell ref="C17:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A28:A33"/>
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="C28:C33"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B40:B43"/>
-    <mergeCell ref="C40:C43"/>
-    <mergeCell ref="C44:C55"/>
-    <mergeCell ref="A44:A55"/>
-    <mergeCell ref="B44:B55"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="A62:A65"/>
-    <mergeCell ref="B62:B65"/>
-    <mergeCell ref="C62:C65"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A3:F3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E24" r:id="rId1"/>
+    <hyperlink ref="F24" r:id="rId2"/>
+    <hyperlink ref="E17" r:id="rId3"/>
+    <hyperlink ref="F34" r:id="rId4"/>
+    <hyperlink ref="F40" r:id="rId5"/>
+    <hyperlink ref="E44" r:id="rId6"/>
+    <hyperlink ref="F44" r:id="rId7"/>
+    <hyperlink ref="E56" r:id="rId8"/>
+    <hyperlink ref="F60" r:id="rId9"/>
+    <hyperlink ref="E62" r:id="rId10"/>
+    <hyperlink ref="E7" r:id="rId11"/>
+    <hyperlink ref="F7" r:id="rId12"/>
+    <hyperlink ref="E13" r:id="rId13"/>
+    <hyperlink ref="F13" r:id="rId14"/>
+    <hyperlink ref="F17" r:id="rId15"/>
+    <hyperlink ref="E28" r:id="rId16"/>
+    <hyperlink ref="F28" r:id="rId17"/>
+    <hyperlink ref="E34" r:id="rId18"/>
+    <hyperlink ref="E37" r:id="rId19"/>
+    <hyperlink ref="F37" r:id="rId20"/>
+    <hyperlink ref="E40" r:id="rId21"/>
+    <hyperlink ref="F56" r:id="rId22"/>
+    <hyperlink ref="E60" r:id="rId23"/>
+    <hyperlink ref="F62" r:id="rId24"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>